<commit_message>
Relation rename change operator + unit test
</commit_message>
<xml_diff>
--- a/resources/TyphonChangeOperatorParameters.xlsx
+++ b/resources/TyphonChangeOperatorParameters.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Documents UNamur\Personnel\Projet TYPHON\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projets\Typhon\workspace\typhon-evolutiontool\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="90">
   <si>
     <t>TyphonML ChangeOperator</t>
   </si>
@@ -273,12 +273,33 @@
   </si>
   <si>
     <t>Either add the source entity in the Change Operator, or in the Relation object.</t>
+  </si>
+  <si>
+    <t>EnableBidirectionalRelation</t>
+  </si>
+  <si>
+    <t>ENABLEOPPOSITE</t>
+  </si>
+  <si>
+    <t>enableOpposite</t>
+  </si>
+  <si>
+    <t>deleteRelationship</t>
+  </si>
+  <si>
+    <t>disableOpposite</t>
+  </si>
+  <si>
+    <t>DisableBidirectionalRelation</t>
+  </si>
+  <si>
+    <t>DISABLEOPPOSITE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -454,7 +475,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -478,13 +499,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -759,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38:F38"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,7 +1229,7 @@
       <c r="G28" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H28" s="17"/>
+      <c r="H28" s="23"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="17"/>
@@ -1195,7 +1245,7 @@
       <c r="G29" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="H29" s="17"/>
+      <c r="H29" s="18"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
@@ -1211,7 +1261,7 @@
       <c r="G30" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H30" s="17"/>
+      <c r="H30" s="18"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
@@ -1325,7 +1375,7 @@
         <v>40</v>
       </c>
       <c r="G37" s="17"/>
-      <c r="H37" s="17" t="s">
+      <c r="H37" s="18" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1341,7 +1391,7 @@
         <v>14</v>
       </c>
       <c r="G38" s="1"/>
-      <c r="H38" s="1" t="s">
+      <c r="H38" s="20" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1365,6 +1415,7 @@
         <v>47</v>
       </c>
       <c r="G39" s="2"/>
+      <c r="H39" s="18"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
@@ -1378,7 +1429,77 @@
         <v>47</v>
       </c>
       <c r="G40" s="5"/>
-      <c r="H40" s="1"/>
+      <c r="H40" s="20"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" t="s">
+        <v>40</v>
+      </c>
+      <c r="D41" t="s">
+        <v>84</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H41" s="18"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F42" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" s="1"/>
+      <c r="H42" s="20"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" t="s">
+        <v>40</v>
+      </c>
+      <c r="D43" t="s">
+        <v>89</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H43" s="18"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Relation change cardinality change operator + unit test
</commit_message>
<xml_diff>
--- a/resources/TyphonChangeOperatorParameters.xlsx
+++ b/resources/TyphonChangeOperatorParameters.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="95">
   <si>
     <t>TyphonML ChangeOperator</t>
   </si>
@@ -300,6 +300,15 @@
   </si>
   <si>
     <t>RenameRelation</t>
+  </si>
+  <si>
+    <t>CHANGECARDINALITY</t>
+  </si>
+  <si>
+    <t>ChangeRelationCardinality</t>
+  </si>
+  <si>
+    <t>cardinality (newCardinality?)</t>
   </si>
 </sst>
 </file>
@@ -815,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1542,6 +1551,31 @@
       <c r="G46" s="1"/>
       <c r="H46" s="20"/>
     </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" t="s">
+        <v>40</v>
+      </c>
+      <c r="D47" t="s">
+        <v>92</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E48" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updates in Typhon change parameters XLS file
</commit_message>
<xml_diff>
--- a/resources/TyphonChangeOperatorParameters.xlsx
+++ b/resources/TyphonChangeOperatorParameters.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="98">
   <si>
     <t>TyphonML ChangeOperator</t>
   </si>
@@ -302,13 +302,22 @@
     <t>RenameRelation</t>
   </si>
   <si>
+    <t>relationToRename</t>
+  </si>
+  <si>
+    <t>newRelationName</t>
+  </si>
+  <si>
     <t>CHANGECARDINALITY</t>
   </si>
   <si>
     <t>ChangeRelationCardinality</t>
   </si>
   <si>
-    <t>cardinality (newCardinality?)</t>
+    <t>newCardinality</t>
+  </si>
+  <si>
+    <t>changeCardinalityInRelation</t>
   </si>
 </sst>
 </file>
@@ -826,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1530,7 +1539,7 @@
         <v>22</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>41</v>
+        <v>92</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>40</v>
@@ -1543,7 +1552,7 @@
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>47</v>
@@ -1552,14 +1561,17 @@
       <c r="H46" s="20"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>97</v>
+      </c>
       <c r="B47" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C47" t="s">
         <v>40</v>
       </c>
       <c r="D47" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>41</v>
@@ -1567,14 +1579,21 @@
       <c r="F47" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="H47" s="18"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E48" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F48" s="2" t="s">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="G48" s="1"/>
+      <c r="H48" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Attributes add and change type change operators + unit tests
</commit_message>
<xml_diff>
--- a/resources/TyphonChangeOperatorParameters.xlsx
+++ b/resources/TyphonChangeOperatorParameters.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="111">
   <si>
     <t>TyphonML ChangeOperator</t>
   </si>
@@ -318,6 +318,45 @@
   </si>
   <si>
     <t>changeCardinalityInRelation</t>
+  </si>
+  <si>
+    <t>addAttribute</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>AddAttribute</t>
+  </si>
+  <si>
+    <t>deleteAttribute</t>
+  </si>
+  <si>
+    <t>RemoveAttribute</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>DataType</t>
+  </si>
+  <si>
+    <t>changeTypeAttribute</t>
+  </si>
+  <si>
+    <t>ChangeAttributeType</t>
+  </si>
+  <si>
+    <t>CHANGETYPE</t>
+  </si>
+  <si>
+    <t>attributeToChange</t>
+  </si>
+  <si>
+    <t>newType</t>
   </si>
 </sst>
 </file>
@@ -833,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,7 +884,7 @@
     <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" customWidth="1"/>
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="53.140625" customWidth="1"/>
@@ -1595,6 +1634,129 @@
       <c r="G48" s="1"/>
       <c r="H48" s="20"/>
     </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" t="s">
+        <v>100</v>
+      </c>
+      <c r="D49" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H49" s="18"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E50" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H50" s="18"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G51" s="1"/>
+      <c r="H51" s="20"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>106</v>
+      </c>
+      <c r="B52" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" t="s">
+        <v>100</v>
+      </c>
+      <c r="D52" t="s">
+        <v>108</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H52" s="18"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E53" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H53" s="18"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G54" s="1"/>
+      <c r="H54" s="20"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>102</v>
+      </c>
+      <c r="B55" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55" t="s">
+        <v>100</v>
+      </c>
+      <c r="D55" t="s">
+        <v>18</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F55" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H55" s="18"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G56" s="1"/>
+      <c r="H56" s="20"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Remove attribute change operator + unit tests
</commit_message>
<xml_diff>
--- a/resources/TyphonChangeOperatorParameters.xlsx
+++ b/resources/TyphonChangeOperatorParameters.xlsx
@@ -323,18 +323,12 @@
     <t>addAttribute</t>
   </si>
   <si>
-    <t>attribute</t>
-  </si>
-  <si>
     <t>Attribute</t>
   </si>
   <si>
     <t>AddAttribute</t>
   </si>
   <si>
-    <t>deleteAttribute</t>
-  </si>
-  <si>
     <t>RemoveAttribute</t>
   </si>
   <si>
@@ -357,6 +351,12 @@
   </si>
   <si>
     <t>newType</t>
+  </si>
+  <si>
+    <t>attributeToRemove</t>
+  </si>
+  <si>
+    <t>removeAttribute</t>
   </si>
 </sst>
 </file>
@@ -875,7 +875,7 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1639,10 +1639,10 @@
         <v>98</v>
       </c>
       <c r="B49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C49" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D49" t="s">
         <v>9</v>
@@ -1657,10 +1657,10 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E50" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H50" s="18"/>
     </row>
@@ -1680,31 +1680,31 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>104</v>
+      </c>
+      <c r="B52" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" t="s">
+        <v>99</v>
+      </c>
+      <c r="D52" t="s">
         <v>106</v>
       </c>
-      <c r="B52" t="s">
+      <c r="E52" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C52" t="s">
-        <v>100</v>
-      </c>
-      <c r="D52" t="s">
-        <v>108</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="F52" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H52" s="18"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E53" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H53" s="18"/>
     </row>
@@ -1724,13 +1724,13 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B55" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C55" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D55" t="s">
         <v>18</v>
@@ -1749,10 +1749,10 @@
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56" s="20"/>

</xml_diff>

<commit_message>
Rename attribute change operator + unit tests
</commit_message>
<xml_diff>
--- a/resources/TyphonChangeOperatorParameters.xlsx
+++ b/resources/TyphonChangeOperatorParameters.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="115">
   <si>
     <t>TyphonML ChangeOperator</t>
   </si>
@@ -357,6 +357,18 @@
   </si>
   <si>
     <t>removeAttribute</t>
+  </si>
+  <si>
+    <t>renameAttribute</t>
+  </si>
+  <si>
+    <t>RenameAttribute</t>
+  </si>
+  <si>
+    <t>attributeToRename</t>
+  </si>
+  <si>
+    <t>newName</t>
   </si>
 </sst>
 </file>
@@ -872,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1757,6 +1769,50 @@
       <c r="G56" s="1"/>
       <c r="H56" s="20"/>
     </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" t="s">
+        <v>112</v>
+      </c>
+      <c r="C57" t="s">
+        <v>99</v>
+      </c>
+      <c r="D57" t="s">
+        <v>22</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H57" s="18"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E58" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H58" s="18"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F59" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G59" s="1"/>
+      <c r="H59" s="20"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Correction of remove relation change operator + unit test
</commit_message>
<xml_diff>
--- a/resources/TyphonChangeOperatorParameters.xlsx
+++ b/resources/TyphonChangeOperatorParameters.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="116">
   <si>
     <t>TyphonML ChangeOperator</t>
   </si>
@@ -369,6 +369,9 @@
   </si>
   <si>
     <t>newName</t>
+  </si>
+  <si>
+    <t>relationToRemove</t>
   </si>
 </sst>
 </file>
@@ -884,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,7 +899,7 @@
     <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" customWidth="1"/>
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="53.140625" customWidth="1"/>
@@ -1471,347 +1474,333 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="E39" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G39" s="1"/>
+      <c r="H39" s="20"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" t="s">
+        <v>40</v>
+      </c>
+      <c r="D40" t="s">
+        <v>84</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H40" s="18"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F41" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="1"/>
+      <c r="H41" s="20"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B42" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42" t="s">
+        <v>89</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H42" s="18"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="20"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" t="s">
+        <v>40</v>
+      </c>
+      <c r="D44" t="s">
+        <v>22</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H44" s="18"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G39" s="2"/>
-      <c r="H39" s="18"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="21" t="s">
+      <c r="G45" s="1"/>
+      <c r="H45" s="20"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" t="s">
+        <v>40</v>
+      </c>
+      <c r="D46" t="s">
+        <v>94</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H46" s="18"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G47" s="1"/>
+      <c r="H47" s="20"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>98</v>
+      </c>
+      <c r="B48" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" t="s">
+        <v>99</v>
+      </c>
+      <c r="D48" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H48" s="18"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E49" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H49" s="18"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F40" s="21" t="s">
+      <c r="F50" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="G40" s="5"/>
-      <c r="H40" s="20"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" t="s">
-        <v>40</v>
-      </c>
-      <c r="D41" t="s">
-        <v>84</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H41" s="18"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="F42" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="G42" s="1"/>
-      <c r="H42" s="20"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="B43" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" t="s">
-        <v>40</v>
-      </c>
-      <c r="D43" t="s">
-        <v>89</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H43" s="18"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="20"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>90</v>
-      </c>
-      <c r="B45" t="s">
-        <v>91</v>
-      </c>
-      <c r="C45" t="s">
-        <v>40</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="G50" s="1"/>
+      <c r="H50" s="20"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>104</v>
+      </c>
+      <c r="B51" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" t="s">
+        <v>99</v>
+      </c>
+      <c r="D51" t="s">
+        <v>106</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H51" s="18"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E52" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H52" s="18"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F53" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G53" s="1"/>
+      <c r="H53" s="20"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>110</v>
+      </c>
+      <c r="B54" t="s">
+        <v>101</v>
+      </c>
+      <c r="C54" t="s">
+        <v>99</v>
+      </c>
+      <c r="D54" t="s">
+        <v>18</v>
+      </c>
+      <c r="E54" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H54" s="18"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G55" s="1"/>
+      <c r="H55" s="20"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>111</v>
+      </c>
+      <c r="B56" t="s">
+        <v>112</v>
+      </c>
+      <c r="C56" t="s">
+        <v>99</v>
+      </c>
+      <c r="D56" t="s">
         <v>22</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H45" s="18"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F46" s="1" t="s">
+      <c r="E56" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H56" s="18"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E57" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F57" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G46" s="1"/>
-      <c r="H46" s="20"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>97</v>
-      </c>
-      <c r="B47" t="s">
-        <v>95</v>
-      </c>
-      <c r="C47" t="s">
-        <v>40</v>
-      </c>
-      <c r="D47" t="s">
-        <v>94</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H47" s="18"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G48" s="1"/>
-      <c r="H48" s="20"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>98</v>
-      </c>
-      <c r="B49" t="s">
-        <v>100</v>
-      </c>
-      <c r="C49" t="s">
-        <v>99</v>
-      </c>
-      <c r="D49" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F49" s="2" t="s">
+      <c r="H57" s="18"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F58" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="H49" s="18"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E50" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H50" s="18"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F51" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="G51" s="1"/>
-      <c r="H51" s="20"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>104</v>
-      </c>
-      <c r="B52" t="s">
-        <v>105</v>
-      </c>
-      <c r="C52" t="s">
-        <v>99</v>
-      </c>
-      <c r="D52" t="s">
-        <v>106</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H52" s="18"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E53" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H53" s="18"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F54" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="G54" s="1"/>
-      <c r="H54" s="20"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>110</v>
-      </c>
-      <c r="B55" t="s">
-        <v>101</v>
-      </c>
-      <c r="C55" t="s">
-        <v>99</v>
-      </c>
-      <c r="D55" t="s">
-        <v>18</v>
-      </c>
-      <c r="E55" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="F55" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="H55" s="18"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G56" s="1"/>
-      <c r="H56" s="20"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>111</v>
-      </c>
-      <c r="B57" t="s">
-        <v>112</v>
-      </c>
-      <c r="C57" t="s">
-        <v>99</v>
-      </c>
-      <c r="D57" t="s">
-        <v>22</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H57" s="18"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E58" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H58" s="18"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F59" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="G59" s="1"/>
-      <c r="H59" s="20"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Enable/disable containment relation change operators review + unit tests
</commit_message>
<xml_diff>
--- a/resources/TyphonChangeOperatorParameters.xlsx
+++ b/resources/TyphonChangeOperatorParameters.xlsx
@@ -902,13 +902,13 @@
   <dimension ref="A1:XFD63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>

</xml_diff>